<commit_message>
Added mana_gov app structure
</commit_message>
<xml_diff>
--- a/backend/mana_algo/mana_algo_inputs/dev_reports/HACKATHON_SHAWN_MANA_HOURS.xlsx
+++ b/backend/mana_algo/mana_algo_inputs/dev_reports/HACKATHON_SHAWN_MANA_HOURS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FYRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -651,12 +651,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -693,7 +699,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -718,6 +724,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -735,7 +745,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -751,7 +761,74 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00A933"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -803,10 +880,10 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2:H4 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.28"/>
@@ -1031,11 +1108,11 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.71"/>
@@ -1213,10 +1290,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2:H4 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.57"/>
@@ -1464,10 +1541,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="H2:H4 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.28"/>
@@ -1756,10 +1833,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="1" sqref="H2:H4 E25"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -2118,16 +2195,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
@@ -2186,11 +2263,11 @@
       <c r="G2" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2234,11 +2311,11 @@
       <c r="G4" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2282,11 +2359,11 @@
       <c r="G6" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="6" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2330,11 +2407,11 @@
       <c r="G8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -2430,7 +2507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -2478,7 +2555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -2574,7 +2651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
@@ -2622,7 +2699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -2645,7 +2722,13 @@
       <c r="H21" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H21"/>
+  <autoFilter ref="A1:H21">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Backend Developer"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2665,10 +2748,10 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.85"/>
@@ -3294,10 +3377,10 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="1" sqref="H2:H4 E27"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
@@ -3309,25 +3392,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -3335,406 +3418,406 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G4" s="7"/>
+      <c r="F4" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7"/>
+      <c r="F8" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G9" s="7"/>
+      <c r="F9" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F10" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7"/>
+      <c r="F10" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G12" s="7"/>
+      <c r="F12" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F14" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G14" s="7"/>
+      <c r="F14" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7"/>
+      <c r="F15" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G16" s="7"/>
+      <c r="F16" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G17" s="7"/>
+      <c r="F17" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F18" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G18" s="7"/>
+      <c r="F18" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G19" s="7"/>
+      <c r="F19" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H20" s="8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -3759,10 +3842,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.43"/>
@@ -3924,10 +4007,10 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="27.42"/>

</xml_diff>